<commit_message>
Entered results for iteration 3
</commit_message>
<xml_diff>
--- a/Results/Project Results Form.xlsx
+++ b/Results/Project Results Form.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="72">
   <si>
     <t>Yes</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>Application Results</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -375,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -417,30 +420,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -457,13 +444,41 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -759,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K151"/>
+  <dimension ref="A1:K152"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A140" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J108" sqref="J108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -847,33 +862,33 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="15.75">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="43" t="s">
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="45" t="s">
+      <c r="H7" s="36"/>
+      <c r="I7" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="46"/>
-      <c r="K7" s="47"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="39"/>
     </row>
     <row r="8" spans="1:11" ht="34.5" customHeight="1">
-      <c r="A8" s="48"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="50"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="41"/>
       <c r="I8" s="7" t="s">
         <v>16</v>
       </c>
@@ -885,13 +900,13 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="13" customFormat="1">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="11"/>
       <c r="G9" s="12"/>
       <c r="H9" s="11"/>
@@ -900,13 +915,13 @@
       <c r="K9" s="17"/>
     </row>
     <row r="10" spans="1:11" s="14" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="15"/>
       <c r="G10" s="19"/>
       <c r="H10" s="15"/>
@@ -915,13 +930,13 @@
       <c r="K10" s="18"/>
     </row>
     <row r="11" spans="1:11" s="14" customFormat="1">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="11"/>
       <c r="G11" s="12"/>
       <c r="H11" s="11"/>
@@ -930,13 +945,13 @@
       <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" s="14" customFormat="1">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="11"/>
       <c r="G12" s="12"/>
       <c r="H12" s="11"/>
@@ -945,13 +960,13 @@
       <c r="K12" s="17"/>
     </row>
     <row r="13" spans="1:11" s="14" customFormat="1">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="11"/>
       <c r="G13" s="12"/>
       <c r="H13" s="11"/>
@@ -973,10 +988,10 @@
       <c r="I15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="51" t="s">
+      <c r="J15" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="52"/>
+      <c r="K15" s="34"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="6"/>
@@ -990,8 +1005,8 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="40"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="43"/>
     </row>
     <row r="17" spans="1:11">
       <c r="C17" s="6"/>
@@ -1003,8 +1018,8 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="40"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="43"/>
     </row>
     <row r="18" spans="1:11">
       <c r="C18" s="6"/>
@@ -1016,8 +1031,8 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="40"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="43"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
@@ -1135,33 +1150,33 @@
       <c r="I52" s="1"/>
     </row>
     <row r="53" spans="1:11" ht="15.75">
-      <c r="A53" s="41" t="s">
+      <c r="A53" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="42"/>
-      <c r="C53" s="42"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="40"/>
-      <c r="G53" s="43" t="s">
+      <c r="B53" s="45"/>
+      <c r="C53" s="45"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="43"/>
+      <c r="G53" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="H53" s="44"/>
-      <c r="I53" s="45" t="s">
+      <c r="H53" s="36"/>
+      <c r="I53" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="J53" s="46"/>
-      <c r="K53" s="47"/>
+      <c r="J53" s="38"/>
+      <c r="K53" s="39"/>
     </row>
     <row r="54" spans="1:11" ht="30">
-      <c r="A54" s="48"/>
-      <c r="B54" s="49"/>
-      <c r="C54" s="49"/>
-      <c r="D54" s="49"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="40"/>
-      <c r="G54" s="48"/>
-      <c r="H54" s="50"/>
+      <c r="A54" s="40"/>
+      <c r="B54" s="42"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="43"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="41"/>
       <c r="I54" s="7" t="s">
         <v>16</v>
       </c>
@@ -1173,13 +1188,13 @@
       </c>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
       <c r="F55" s="11"/>
       <c r="G55" s="12"/>
       <c r="H55" s="11"/>
@@ -1188,13 +1203,13 @@
       <c r="K55" s="17"/>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="37" t="s">
+      <c r="A56" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="B56" s="38"/>
-      <c r="C56" s="38"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="38"/>
+      <c r="B56" s="47"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="47"/>
+      <c r="E56" s="47"/>
       <c r="F56" s="15"/>
       <c r="G56" s="19"/>
       <c r="H56" s="15"/>
@@ -1216,10 +1231,10 @@
       <c r="I58" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J58" s="51" t="s">
+      <c r="J58" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="K58" s="52"/>
+      <c r="K58" s="34"/>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="6"/>
@@ -1233,8 +1248,8 @@
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
       <c r="I59" s="3"/>
-      <c r="J59" s="39"/>
-      <c r="K59" s="40"/>
+      <c r="J59" s="48"/>
+      <c r="K59" s="43"/>
     </row>
     <row r="60" spans="1:11">
       <c r="C60" s="6"/>
@@ -1246,8 +1261,8 @@
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="3"/>
-      <c r="J60" s="39"/>
-      <c r="K60" s="40"/>
+      <c r="J60" s="48"/>
+      <c r="K60" s="43"/>
     </row>
     <row r="61" spans="1:11">
       <c r="C61" s="6"/>
@@ -1259,8 +1274,8 @@
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="3"/>
-      <c r="J61" s="39"/>
-      <c r="K61" s="40"/>
+      <c r="J61" s="48"/>
+      <c r="K61" s="43"/>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="1" t="s">
@@ -1442,14 +1457,18 @@
         <v>20</v>
       </c>
       <c r="B98" s="1"/>
-      <c r="C98" s="3"/>
+      <c r="C98" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="99" spans="1:11">
       <c r="A99" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B99" s="1"/>
-      <c r="C99" s="3"/>
+      <c r="C99" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="100" spans="1:11">
       <c r="B100" s="1"/>
@@ -1462,33 +1481,33 @@
       <c r="I100" s="1"/>
     </row>
     <row r="101" spans="1:11" ht="15.75">
-      <c r="A101" s="41" t="s">
+      <c r="A101" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B101" s="42"/>
-      <c r="C101" s="42"/>
-      <c r="D101" s="36"/>
-      <c r="E101" s="36"/>
-      <c r="F101" s="40"/>
-      <c r="G101" s="43" t="s">
+      <c r="B101" s="45"/>
+      <c r="C101" s="45"/>
+      <c r="D101" s="32"/>
+      <c r="E101" s="32"/>
+      <c r="F101" s="43"/>
+      <c r="G101" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="H101" s="44"/>
-      <c r="I101" s="45" t="s">
+      <c r="H101" s="36"/>
+      <c r="I101" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="J101" s="46"/>
-      <c r="K101" s="47"/>
+      <c r="J101" s="38"/>
+      <c r="K101" s="39"/>
     </row>
     <row r="102" spans="1:11" ht="30">
-      <c r="A102" s="48"/>
-      <c r="B102" s="49"/>
-      <c r="C102" s="49"/>
-      <c r="D102" s="49"/>
-      <c r="E102" s="49"/>
-      <c r="F102" s="40"/>
-      <c r="G102" s="48"/>
-      <c r="H102" s="50"/>
+      <c r="A102" s="40"/>
+      <c r="B102" s="42"/>
+      <c r="C102" s="42"/>
+      <c r="D102" s="42"/>
+      <c r="E102" s="42"/>
+      <c r="F102" s="43"/>
+      <c r="G102" s="40"/>
+      <c r="H102" s="41"/>
       <c r="I102" s="7" t="s">
         <v>16</v>
       </c>
@@ -1500,34 +1519,48 @@
       </c>
     </row>
     <row r="103" spans="1:11">
-      <c r="A103" s="35" t="s">
+      <c r="A103" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B103" s="36"/>
-      <c r="C103" s="36"/>
-      <c r="D103" s="36"/>
-      <c r="E103" s="36"/>
+      <c r="B103" s="32"/>
+      <c r="C103" s="32"/>
+      <c r="D103" s="32"/>
+      <c r="E103" s="32"/>
       <c r="F103" s="11"/>
-      <c r="G103" s="12"/>
-      <c r="H103" s="11"/>
-      <c r="I103" s="17"/>
-      <c r="J103" s="17"/>
-      <c r="K103" s="17"/>
+      <c r="G103" s="53">
+        <v>0</v>
+      </c>
+      <c r="H103" s="54"/>
+      <c r="I103" s="17">
+        <v>4</v>
+      </c>
+      <c r="J103" s="17">
+        <v>3</v>
+      </c>
+      <c r="K103" s="17">
+        <v>38</v>
+      </c>
     </row>
     <row r="104" spans="1:11">
-      <c r="A104" s="37" t="s">
+      <c r="A104" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="B104" s="38"/>
-      <c r="C104" s="38"/>
-      <c r="D104" s="38"/>
-      <c r="E104" s="38"/>
+      <c r="B104" s="47"/>
+      <c r="C104" s="47"/>
+      <c r="D104" s="47"/>
+      <c r="E104" s="47"/>
       <c r="F104" s="15"/>
-      <c r="G104" s="19"/>
-      <c r="H104" s="15"/>
-      <c r="I104" s="18"/>
-      <c r="J104" s="18"/>
-      <c r="K104" s="18"/>
+      <c r="G104" s="55"/>
+      <c r="H104" s="56"/>
+      <c r="I104" s="18">
+        <v>10</v>
+      </c>
+      <c r="J104" s="18">
+        <v>2</v>
+      </c>
+      <c r="K104" s="18">
+        <v>41</v>
+      </c>
     </row>
     <row r="106" spans="1:11" ht="18.75">
       <c r="A106" s="21" t="s">
@@ -1555,18 +1588,20 @@
       <c r="F107" s="6"/>
       <c r="G107" s="6"/>
       <c r="H107" s="23"/>
-      <c r="I107" s="33"/>
-      <c r="J107" s="33"/>
+      <c r="I107" s="51"/>
+      <c r="J107" s="51"/>
     </row>
     <row r="108" spans="1:11">
-      <c r="C108" s="3"/>
+      <c r="C108" s="3">
+        <v>3</v>
+      </c>
       <c r="D108" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E108" s="3"/>
-      <c r="F108" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="E108" s="3">
+        <v>3</v>
+      </c>
+      <c r="F108" s="1"/>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" s="10" t="s">
@@ -1574,13 +1609,23 @@
       </c>
     </row>
     <row r="111" spans="1:11">
-      <c r="C111" s="3"/>
+      <c r="C111" s="3">
+        <v>2</v>
+      </c>
       <c r="D111" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E111" s="3"/>
+      <c r="E111" s="3">
+        <v>2</v>
+      </c>
       <c r="F111" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="I111" s="3">
+        <v>2</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="112" spans="1:11">
@@ -1589,11 +1634,15 @@
       </c>
     </row>
     <row r="113" spans="1:11">
-      <c r="C113" s="3"/>
+      <c r="C113" s="3">
+        <v>3</v>
+      </c>
       <c r="D113" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E113" s="3"/>
+      <c r="E113" s="3">
+        <v>3</v>
+      </c>
       <c r="F113" s="1" t="s">
         <v>6</v>
       </c>
@@ -1619,22 +1668,24 @@
       <c r="J115" s="25"/>
       <c r="K115" s="25"/>
     </row>
-    <row r="116" spans="1:11">
-      <c r="A116" s="34" t="s">
+    <row r="116" spans="1:11" ht="31.5" customHeight="1">
+      <c r="A116" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="B116" s="32"/>
-      <c r="C116" s="32"/>
-      <c r="D116" s="32"/>
-      <c r="E116" s="32"/>
-      <c r="F116" s="32"/>
-      <c r="G116" s="32"/>
-      <c r="H116" s="32"/>
-      <c r="I116" s="32"/>
-      <c r="J116" s="32"/>
+      <c r="B116" s="50"/>
+      <c r="C116" s="50"/>
+      <c r="D116" s="50"/>
+      <c r="E116" s="50"/>
+      <c r="F116" s="50"/>
+      <c r="G116" s="50"/>
+      <c r="H116" s="50"/>
+      <c r="I116" s="50"/>
+      <c r="J116" s="50"/>
     </row>
     <row r="117" spans="1:11">
-      <c r="C117" s="3"/>
+      <c r="C117" s="3">
+        <v>5</v>
+      </c>
       <c r="D117" s="1" t="s">
         <v>0</v>
       </c>
@@ -1642,8 +1693,12 @@
       <c r="F117" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G117" s="6"/>
-      <c r="H117" s="6"/>
+      <c r="G117" s="3">
+        <v>1</v>
+      </c>
+      <c r="H117" s="10" t="s">
+        <v>71</v>
+      </c>
       <c r="I117" s="6"/>
       <c r="J117" s="6"/>
     </row>
@@ -1653,11 +1708,15 @@
       </c>
     </row>
     <row r="120" spans="1:11">
-      <c r="C120" s="3"/>
+      <c r="C120" s="3">
+        <v>3</v>
+      </c>
       <c r="D120" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E120" s="3"/>
+      <c r="E120" s="3">
+        <v>3</v>
+      </c>
       <c r="F120" s="1" t="s">
         <v>53</v>
       </c>
@@ -1672,11 +1731,15 @@
       </c>
     </row>
     <row r="123" spans="1:11">
-      <c r="C123" s="3"/>
+      <c r="C123" s="3">
+        <v>3</v>
+      </c>
       <c r="D123" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E123" s="3"/>
+      <c r="E123" s="3">
+        <v>3</v>
+      </c>
       <c r="F123" s="1" t="s">
         <v>53</v>
       </c>
@@ -1691,7 +1754,9 @@
       </c>
     </row>
     <row r="126" spans="1:11">
-      <c r="C126" s="3"/>
+      <c r="C126" s="3">
+        <v>1</v>
+      </c>
       <c r="D126" s="1" t="s">
         <v>0</v>
       </c>
@@ -1699,8 +1764,12 @@
       <c r="F126" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G126" s="6"/>
-      <c r="H126" s="6"/>
+      <c r="G126" s="3">
+        <v>5</v>
+      </c>
+      <c r="H126" s="10" t="s">
+        <v>71</v>
+      </c>
       <c r="I126" s="6"/>
       <c r="J126" s="6"/>
     </row>
@@ -1710,11 +1779,15 @@
       </c>
     </row>
     <row r="129" spans="1:11">
-      <c r="C129" s="3"/>
+      <c r="C129" s="3">
+        <v>3</v>
+      </c>
       <c r="D129" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E129" s="3"/>
+      <c r="E129" s="3">
+        <v>3</v>
+      </c>
       <c r="F129" s="1" t="s">
         <v>53</v>
       </c>
@@ -1724,21 +1797,23 @@
       <c r="J129" s="6"/>
     </row>
     <row r="131" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A131" s="31" t="s">
+      <c r="A131" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="B131" s="31"/>
-      <c r="C131" s="31"/>
-      <c r="D131" s="31"/>
-      <c r="E131" s="31"/>
-      <c r="F131" s="31"/>
-      <c r="G131" s="31"/>
-      <c r="H131" s="31"/>
-      <c r="I131" s="31"/>
-      <c r="J131" s="31"/>
+      <c r="B131" s="49"/>
+      <c r="C131" s="49"/>
+      <c r="D131" s="49"/>
+      <c r="E131" s="49"/>
+      <c r="F131" s="49"/>
+      <c r="G131" s="49"/>
+      <c r="H131" s="49"/>
+      <c r="I131" s="49"/>
+      <c r="J131" s="49"/>
     </row>
     <row r="132" spans="1:11">
-      <c r="C132" s="3"/>
+      <c r="C132" s="3">
+        <v>6</v>
+      </c>
       <c r="D132" s="1" t="s">
         <v>0</v>
       </c>
@@ -1777,25 +1852,29 @@
       <c r="K134" s="25"/>
     </row>
     <row r="135" spans="1:11" ht="33" customHeight="1">
-      <c r="A135" s="31" t="s">
+      <c r="A135" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="B135" s="32"/>
-      <c r="C135" s="32"/>
-      <c r="D135" s="32"/>
-      <c r="E135" s="32"/>
-      <c r="F135" s="32"/>
-      <c r="G135" s="32"/>
-      <c r="H135" s="32"/>
-      <c r="I135" s="32"/>
-      <c r="J135" s="32"/>
+      <c r="B135" s="50"/>
+      <c r="C135" s="50"/>
+      <c r="D135" s="50"/>
+      <c r="E135" s="50"/>
+      <c r="F135" s="50"/>
+      <c r="G135" s="50"/>
+      <c r="H135" s="50"/>
+      <c r="I135" s="50"/>
+      <c r="J135" s="50"/>
     </row>
     <row r="136" spans="1:11">
-      <c r="C136" s="3"/>
+      <c r="C136" s="3">
+        <v>2</v>
+      </c>
       <c r="D136" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E136" s="3"/>
+      <c r="E136" s="3">
+        <v>4</v>
+      </c>
       <c r="F136" s="1" t="s">
         <v>53</v>
       </c>
@@ -1814,102 +1893,106 @@
       <c r="I137" s="6"/>
       <c r="J137" s="6"/>
     </row>
-    <row r="138" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A138" s="31" t="s">
+    <row r="138" spans="1:11">
+      <c r="C138" s="6"/>
+      <c r="D138" s="1"/>
+      <c r="E138" s="6"/>
+      <c r="F138" s="1"/>
+      <c r="G138" s="6"/>
+      <c r="H138" s="6"/>
+      <c r="I138" s="6"/>
+      <c r="J138" s="6"/>
+    </row>
+    <row r="139" spans="1:11" ht="29.25" customHeight="1">
+      <c r="A139" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B138" s="32"/>
-      <c r="C138" s="32"/>
-      <c r="D138" s="32"/>
-      <c r="E138" s="32"/>
-      <c r="F138" s="32"/>
-      <c r="G138" s="32"/>
-      <c r="H138" s="32"/>
-      <c r="I138" s="32"/>
-      <c r="J138" s="32"/>
-    </row>
-    <row r="139" spans="1:11">
-      <c r="C139" s="3"/>
-      <c r="D139" s="1" t="s">
+      <c r="B139" s="50"/>
+      <c r="C139" s="50"/>
+      <c r="D139" s="50"/>
+      <c r="E139" s="50"/>
+      <c r="F139" s="50"/>
+      <c r="G139" s="50"/>
+      <c r="H139" s="50"/>
+      <c r="I139" s="50"/>
+      <c r="J139" s="50"/>
+    </row>
+    <row r="140" spans="1:11">
+      <c r="C140" s="3">
+        <v>5</v>
+      </c>
+      <c r="D140" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E139" s="3"/>
-      <c r="F139" s="1" t="s">
+      <c r="E140" s="3">
+        <v>1</v>
+      </c>
+      <c r="F140" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G139" s="6"/>
-      <c r="H139" s="6"/>
-      <c r="I139" s="6"/>
-      <c r="J139" s="6"/>
-    </row>
-    <row r="140" spans="1:11" ht="18.75">
-      <c r="A140" s="24" t="s">
+      <c r="G140" s="6"/>
+      <c r="H140" s="6"/>
+      <c r="I140" s="6"/>
+      <c r="J140" s="6"/>
+    </row>
+    <row r="141" spans="1:11" ht="18.75">
+      <c r="A141" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B140" s="24"/>
-      <c r="C140" s="25"/>
-      <c r="D140" s="25"/>
-      <c r="E140" s="25"/>
-      <c r="F140" s="25"/>
-      <c r="G140" s="25"/>
-      <c r="H140" s="25"/>
-      <c r="I140" s="25"/>
-      <c r="J140" s="25"/>
-      <c r="K140" s="25"/>
-    </row>
-    <row r="141" spans="1:11" ht="61.5" customHeight="1">
-      <c r="A141" s="31" t="s">
+      <c r="B141" s="24"/>
+      <c r="C141" s="25"/>
+      <c r="D141" s="25"/>
+      <c r="E141" s="25"/>
+      <c r="F141" s="25"/>
+      <c r="G141" s="25"/>
+      <c r="H141" s="25"/>
+      <c r="I141" s="25"/>
+      <c r="J141" s="25"/>
+      <c r="K141" s="25"/>
+    </row>
+    <row r="142" spans="1:11" ht="61.5" customHeight="1">
+      <c r="A142" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B141" s="31"/>
-      <c r="C141" s="31"/>
-      <c r="D141" s="31"/>
-      <c r="E141" s="31"/>
-      <c r="F141" s="31"/>
-      <c r="G141" s="31"/>
-      <c r="H141" s="31"/>
-      <c r="I141" s="31"/>
-      <c r="J141" s="31"/>
-    </row>
-    <row r="142" spans="1:11">
-      <c r="C142" s="3"/>
-      <c r="D142" s="1" t="s">
+      <c r="B142" s="49"/>
+      <c r="C142" s="49"/>
+      <c r="D142" s="49"/>
+      <c r="E142" s="49"/>
+      <c r="F142" s="49"/>
+      <c r="G142" s="49"/>
+      <c r="H142" s="49"/>
+      <c r="I142" s="49"/>
+      <c r="J142" s="49"/>
+    </row>
+    <row r="143" spans="1:11">
+      <c r="C143" s="3">
+        <v>4</v>
+      </c>
+      <c r="D143" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E142" s="3"/>
-      <c r="F142" s="1" t="s">
+      <c r="E143" s="3">
+        <v>2</v>
+      </c>
+      <c r="F143" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G142" s="6"/>
-      <c r="H142" s="6"/>
-      <c r="I142" s="6"/>
-      <c r="J142" s="6"/>
-    </row>
-    <row r="144" spans="1:11">
-      <c r="A144" s="1" t="s">
+      <c r="G143" s="6"/>
+      <c r="H143" s="6"/>
+      <c r="I143" s="6"/>
+      <c r="J143" s="6"/>
+    </row>
+    <row r="145" spans="1:10">
+      <c r="A145" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="145" spans="1:10">
-      <c r="A145" s="6"/>
-      <c r="B145" s="6"/>
-      <c r="C145" s="3"/>
-      <c r="D145" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E145" s="6"/>
-      <c r="F145" s="10"/>
-      <c r="G145" s="6"/>
-      <c r="H145" s="6"/>
-      <c r="I145" s="6"/>
-      <c r="J145" s="6"/>
     </row>
     <row r="146" spans="1:10">
       <c r="A146" s="6"/>
       <c r="B146" s="6"/>
       <c r="C146" s="3"/>
       <c r="D146" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E146" s="6"/>
       <c r="F146" s="10"/>
@@ -1921,9 +2004,11 @@
     <row r="147" spans="1:10">
       <c r="A147" s="6"/>
       <c r="B147" s="6"/>
-      <c r="C147" s="3"/>
+      <c r="C147" s="3">
+        <v>1</v>
+      </c>
       <c r="D147" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E147" s="6"/>
       <c r="F147" s="10"/>
@@ -1937,7 +2022,7 @@
       <c r="B148" s="6"/>
       <c r="C148" s="3"/>
       <c r="D148" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E148" s="6"/>
       <c r="F148" s="10"/>
@@ -1946,36 +2031,86 @@
       <c r="I148" s="6"/>
       <c r="J148" s="6"/>
     </row>
-    <row r="150" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A150" s="31" t="s">
+    <row r="149" spans="1:10">
+      <c r="A149" s="6"/>
+      <c r="B149" s="6"/>
+      <c r="C149" s="3">
+        <v>5</v>
+      </c>
+      <c r="D149" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E149" s="6"/>
+      <c r="F149" s="10"/>
+      <c r="G149" s="6"/>
+      <c r="H149" s="6"/>
+      <c r="I149" s="6"/>
+      <c r="J149" s="6"/>
+    </row>
+    <row r="151" spans="1:10" ht="32.25" customHeight="1">
+      <c r="A151" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="B150" s="32"/>
-      <c r="C150" s="32"/>
-      <c r="D150" s="32"/>
-      <c r="E150" s="32"/>
-      <c r="F150" s="32"/>
-      <c r="G150" s="32"/>
-      <c r="H150" s="32"/>
-      <c r="I150" s="32"/>
-      <c r="J150" s="32"/>
-    </row>
-    <row r="151" spans="1:10">
-      <c r="C151" s="3"/>
-      <c r="D151" s="1" t="s">
+      <c r="B151" s="50"/>
+      <c r="C151" s="50"/>
+      <c r="D151" s="50"/>
+      <c r="E151" s="50"/>
+      <c r="F151" s="50"/>
+      <c r="G151" s="50"/>
+      <c r="H151" s="50"/>
+      <c r="I151" s="50"/>
+      <c r="J151" s="50"/>
+    </row>
+    <row r="152" spans="1:10">
+      <c r="C152" s="3">
+        <v>4</v>
+      </c>
+      <c r="D152" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E151" s="3"/>
-      <c r="F151" s="1" t="s">
+      <c r="E152" s="3">
+        <v>2</v>
+      </c>
+      <c r="F152" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G151" s="6"/>
-      <c r="H151" s="6"/>
-      <c r="I151" s="6"/>
-      <c r="J151" s="6"/>
+      <c r="G152" s="6"/>
+      <c r="H152" s="6"/>
+      <c r="I152" s="6"/>
+      <c r="J152" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="41">
+    <mergeCell ref="A139:J139"/>
+    <mergeCell ref="A142:J142"/>
+    <mergeCell ref="A151:J151"/>
+    <mergeCell ref="I107:J107"/>
+    <mergeCell ref="A116:J116"/>
+    <mergeCell ref="A131:J131"/>
+    <mergeCell ref="A135:J135"/>
+    <mergeCell ref="A103:E103"/>
+    <mergeCell ref="A104:E104"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="A101:F101"/>
+    <mergeCell ref="G101:H101"/>
+    <mergeCell ref="I101:K101"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="G102:H102"/>
+    <mergeCell ref="G103:H103"/>
+    <mergeCell ref="G104:H104"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A56:E56"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="I53:K53"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="J15:K15"/>
@@ -1987,34 +2122,6 @@
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A11:E11"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="I53:K53"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="J60:K60"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A56:E56"/>
-    <mergeCell ref="A103:E103"/>
-    <mergeCell ref="A104:E104"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="A101:F101"/>
-    <mergeCell ref="G101:H101"/>
-    <mergeCell ref="I101:K101"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="G102:H102"/>
-    <mergeCell ref="A138:J138"/>
-    <mergeCell ref="A141:J141"/>
-    <mergeCell ref="A150:J150"/>
-    <mergeCell ref="I107:J107"/>
-    <mergeCell ref="A116:J116"/>
-    <mergeCell ref="A131:J131"/>
-    <mergeCell ref="A135:J135"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes to results of surveys
</commit_message>
<xml_diff>
--- a/Results/Project Results Form.xlsx
+++ b/Results/Project Results Form.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="75">
   <si>
     <t>Yes</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Section 4 - Visual Feedback - Highlighting</t>
   </si>
   <si>
-    <t>Spoken Link Name</t>
-  </si>
-  <si>
     <t>Verbal</t>
   </si>
   <si>
@@ -232,6 +229,18 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>name ref</t>
+  </si>
+  <si>
+    <t>both</t>
+  </si>
+  <si>
+    <t>not sure</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -378,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -393,7 +402,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -420,7 +428,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -428,6 +435,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -444,30 +479,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -776,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K152"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J108" sqref="J108"/>
+    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="K95" sqref="A1:K95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -795,19 +808,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
+      <c r="A1" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
     </row>
     <row r="2" spans="1:11" ht="18.75">
       <c r="A2" s="8" t="s">
@@ -824,32 +837,36 @@
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="1:11" s="16" customFormat="1" ht="18.75">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
+    <row r="3" spans="1:11" s="15" customFormat="1" ht="18.75">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="B6" s="1"/>
@@ -862,33 +879,33 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="15.75">
-      <c r="A7" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="35" t="s">
+      <c r="A7" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="36"/>
-      <c r="I7" s="37" t="s">
+      <c r="H7" s="48"/>
+      <c r="I7" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="38"/>
-      <c r="K7" s="39"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="51"/>
     </row>
     <row r="8" spans="1:11" ht="34.5" customHeight="1">
-      <c r="A8" s="40"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="41"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="54"/>
       <c r="I8" s="7" t="s">
         <v>16</v>
       </c>
@@ -899,80 +916,120 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="13" customFormat="1">
-      <c r="A9" s="31" t="s">
+    <row r="9" spans="1:11" s="12" customFormat="1">
+      <c r="A9" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-    </row>
-    <row r="10" spans="1:11" s="14" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="46" t="s">
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="35">
+        <v>2</v>
+      </c>
+      <c r="H9" s="30"/>
+      <c r="I9" s="16">
+        <v>2</v>
+      </c>
+      <c r="J9" s="16">
+        <v>0</v>
+      </c>
+      <c r="K9" s="16">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="13" customFormat="1" ht="15" customHeight="1">
+      <c r="A10" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-    </row>
-    <row r="11" spans="1:11" s="14" customFormat="1">
-      <c r="A11" s="31" t="s">
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="18">
+        <v>2</v>
+      </c>
+      <c r="H10" s="34"/>
+      <c r="I10" s="17">
+        <v>1</v>
+      </c>
+      <c r="J10" s="17">
+        <v>1</v>
+      </c>
+      <c r="K10" s="17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="13" customFormat="1">
+      <c r="A11" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-    </row>
-    <row r="12" spans="1:11" s="14" customFormat="1">
-      <c r="A12" s="31" t="s">
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="35">
+        <v>1</v>
+      </c>
+      <c r="H11" s="30"/>
+      <c r="I11" s="16">
+        <v>0</v>
+      </c>
+      <c r="J11" s="16">
+        <v>0</v>
+      </c>
+      <c r="K11" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="13" customFormat="1">
+      <c r="A12" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-    </row>
-    <row r="13" spans="1:11" s="14" customFormat="1">
-      <c r="A13" s="31" t="s">
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="35">
+        <v>2</v>
+      </c>
+      <c r="H12" s="30"/>
+      <c r="I12" s="16">
+        <v>0</v>
+      </c>
+      <c r="J12" s="16">
+        <v>1</v>
+      </c>
+      <c r="K12" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="13" customFormat="1">
+      <c r="A13" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="35">
+        <v>0</v>
+      </c>
+      <c r="H13" s="30"/>
+      <c r="I13" s="16">
+        <v>3</v>
+      </c>
+      <c r="J13" s="16">
+        <v>2</v>
+      </c>
+      <c r="K13" s="16">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="10" t="s">
@@ -988,10 +1045,12 @@
       <c r="I15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="34"/>
+      <c r="J15" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="K15" s="32" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="6"/>
@@ -1004,9 +1063,15 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="43"/>
+      <c r="I16" s="3">
+        <v>4</v>
+      </c>
+      <c r="J16" s="35">
+        <v>2</v>
+      </c>
+      <c r="K16" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:11">
       <c r="C17" s="6"/>
@@ -1017,9 +1082,15 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="43"/>
+      <c r="I17" s="3">
+        <v>2</v>
+      </c>
+      <c r="J17" s="35">
+        <v>4</v>
+      </c>
+      <c r="K17" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:11">
       <c r="C18" s="6"/>
@@ -1030,13 +1101,19 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="43"/>
+      <c r="I18" s="3">
+        <v>4</v>
+      </c>
+      <c r="J18" s="35">
+        <v>2</v>
+      </c>
+      <c r="K18" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1044,24 +1121,30 @@
       <c r="D21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1"/>
       <c r="D22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="3"/>
+      <c r="F22" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23" s="10"/>
-      <c r="F23" s="5"/>
+      <c r="F23" s="5">
+        <v>2</v>
+      </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="6"/>
@@ -1070,36 +1153,44 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="D26" s="19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="D26" s="20" t="s">
+      <c r="H26" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="D27" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="D27" s="20" t="s">
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="D28" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="D28" s="20" t="s">
+      <c r="H28" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="D29" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="D29" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29" s="3"/>
+      <c r="H29" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="48" spans="1:11" ht="18.75">
       <c r="A48" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="9"/>
@@ -1112,32 +1203,36 @@
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
     </row>
-    <row r="49" spans="1:11" s="16" customFormat="1" ht="18.75">
-      <c r="A49" s="28"/>
-      <c r="B49" s="28"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="30"/>
+    <row r="49" spans="1:11" s="15" customFormat="1" ht="18.75">
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="29"/>
+      <c r="K49" s="29"/>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B50" s="1"/>
-      <c r="C50" s="3"/>
+      <c r="C50" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B51" s="1"/>
-      <c r="C51" s="3"/>
+      <c r="C51" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="52" spans="1:11">
       <c r="B52" s="1"/>
@@ -1150,33 +1245,33 @@
       <c r="I52" s="1"/>
     </row>
     <row r="53" spans="1:11" ht="15.75">
-      <c r="A53" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="B53" s="45"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="35" t="s">
+      <c r="A53" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="46"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="41"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="H53" s="36"/>
-      <c r="I53" s="37" t="s">
+      <c r="H53" s="48"/>
+      <c r="I53" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="J53" s="38"/>
-      <c r="K53" s="39"/>
+      <c r="J53" s="50"/>
+      <c r="K53" s="51"/>
     </row>
     <row r="54" spans="1:11" ht="30">
-      <c r="A54" s="40"/>
-      <c r="B54" s="42"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="42"/>
-      <c r="F54" s="43"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="41"/>
+      <c r="A54" s="52"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="52"/>
+      <c r="H54" s="54"/>
       <c r="I54" s="7" t="s">
         <v>16</v>
       </c>
@@ -1188,34 +1283,42 @@
       </c>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B55" s="32"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="17"/>
-      <c r="J55" s="17"/>
-      <c r="K55" s="17"/>
+      <c r="B55" s="41"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="41"/>
+      <c r="E55" s="41"/>
+      <c r="F55" s="30"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="30"/>
+      <c r="I55" s="16">
+        <v>2</v>
+      </c>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16">
+        <v>18</v>
+      </c>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="46" t="s">
+      <c r="A56" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B56" s="47"/>
-      <c r="C56" s="47"/>
-      <c r="D56" s="47"/>
-      <c r="E56" s="47"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="15"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="18"/>
-      <c r="K56" s="18"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="34"/>
+      <c r="I56" s="17">
+        <v>0</v>
+      </c>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17">
+        <v>12</v>
+      </c>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="10" t="s">
@@ -1231,10 +1334,12 @@
       <c r="I58" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J58" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="K58" s="34"/>
+      <c r="J58" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="K58" s="32" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="6"/>
@@ -1247,9 +1352,15 @@
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="48"/>
-      <c r="K59" s="43"/>
+      <c r="I59" s="3">
+        <v>1</v>
+      </c>
+      <c r="J59" s="35">
+        <v>1</v>
+      </c>
+      <c r="K59" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="60" spans="1:11">
       <c r="C60" s="6"/>
@@ -1261,8 +1372,12 @@
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="3"/>
-      <c r="J60" s="48"/>
-      <c r="K60" s="43"/>
+      <c r="J60" s="35">
+        <v>2</v>
+      </c>
+      <c r="K60" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="61" spans="1:11">
       <c r="C61" s="6"/>
@@ -1273,24 +1388,30 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="48"/>
-      <c r="K61" s="43"/>
+      <c r="I61" s="3">
+        <v>1</v>
+      </c>
+      <c r="J61" s="35">
+        <v>1</v>
+      </c>
+      <c r="K61" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="1"/>
       <c r="C65" s="3"/>
       <c r="D65" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -1300,18 +1421,20 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="1"/>
-      <c r="C68" s="3"/>
+      <c r="C68" s="3">
+        <v>3</v>
+      </c>
       <c r="D68" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -1319,12 +1442,14 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="1"/>
-      <c r="C71" s="3"/>
+      <c r="C71" s="3">
+        <v>3</v>
+      </c>
       <c r="D71" s="1" t="s">
         <v>0</v>
       </c>
@@ -1338,16 +1463,18 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I73" s="6"/>
       <c r="J73" s="6"/>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="1"/>
-      <c r="C74" s="3"/>
+      <c r="C74" s="3">
+        <v>3</v>
+      </c>
       <c r="D74" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F74" s="6"/>
       <c r="J74" s="6"/>
@@ -1356,7 +1483,7 @@
       <c r="A75" s="1"/>
       <c r="C75" s="3"/>
       <c r="D75" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F75" s="6"/>
       <c r="J75" s="6"/>
@@ -1365,7 +1492,7 @@
       <c r="A76" s="1"/>
       <c r="C76" s="3"/>
       <c r="D76" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E76" s="10"/>
       <c r="F76" s="6"/>
@@ -1373,27 +1500,37 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="79" spans="1:10">
-      <c r="C79" s="3"/>
-      <c r="D79" s="20" t="s">
+      <c r="C79" s="3">
+        <v>1</v>
+      </c>
+      <c r="D79" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="I79" s="3">
+        <v>2</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="18.75" customHeight="1">
       <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
+      <c r="D82" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
@@ -1426,7 +1563,7 @@
     </row>
     <row r="96" spans="1:11" ht="18.75">
       <c r="A96" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B96" s="8"/>
       <c r="C96" s="9"/>
@@ -1439,18 +1576,18 @@
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
     </row>
-    <row r="97" spans="1:11" s="16" customFormat="1" ht="18.75">
-      <c r="A97" s="28"/>
-      <c r="B97" s="28"/>
-      <c r="C97" s="29"/>
-      <c r="D97" s="30"/>
-      <c r="E97" s="30"/>
-      <c r="F97" s="30"/>
-      <c r="G97" s="30"/>
-      <c r="H97" s="30"/>
-      <c r="I97" s="30"/>
-      <c r="J97" s="30"/>
-      <c r="K97" s="30"/>
+    <row r="97" spans="1:11" s="15" customFormat="1" ht="18.75">
+      <c r="A97" s="27"/>
+      <c r="B97" s="27"/>
+      <c r="C97" s="28"/>
+      <c r="D97" s="29"/>
+      <c r="E97" s="29"/>
+      <c r="F97" s="29"/>
+      <c r="G97" s="29"/>
+      <c r="H97" s="29"/>
+      <c r="I97" s="29"/>
+      <c r="J97" s="29"/>
+      <c r="K97" s="29"/>
     </row>
     <row r="98" spans="1:11">
       <c r="A98" s="1" t="s">
@@ -1481,33 +1618,33 @@
       <c r="I100" s="1"/>
     </row>
     <row r="101" spans="1:11" ht="15.75">
-      <c r="A101" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="B101" s="45"/>
-      <c r="C101" s="45"/>
-      <c r="D101" s="32"/>
-      <c r="E101" s="32"/>
-      <c r="F101" s="43"/>
-      <c r="G101" s="35" t="s">
+      <c r="A101" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B101" s="46"/>
+      <c r="C101" s="46"/>
+      <c r="D101" s="41"/>
+      <c r="E101" s="41"/>
+      <c r="F101" s="44"/>
+      <c r="G101" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="H101" s="36"/>
-      <c r="I101" s="37" t="s">
+      <c r="H101" s="48"/>
+      <c r="I101" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="J101" s="38"/>
-      <c r="K101" s="39"/>
+      <c r="J101" s="50"/>
+      <c r="K101" s="51"/>
     </row>
     <row r="102" spans="1:11" ht="30">
-      <c r="A102" s="40"/>
-      <c r="B102" s="42"/>
-      <c r="C102" s="42"/>
-      <c r="D102" s="42"/>
-      <c r="E102" s="42"/>
-      <c r="F102" s="43"/>
-      <c r="G102" s="40"/>
-      <c r="H102" s="41"/>
+      <c r="A102" s="52"/>
+      <c r="B102" s="53"/>
+      <c r="C102" s="53"/>
+      <c r="D102" s="53"/>
+      <c r="E102" s="53"/>
+      <c r="F102" s="44"/>
+      <c r="G102" s="52"/>
+      <c r="H102" s="54"/>
       <c r="I102" s="7" t="s">
         <v>16</v>
       </c>
@@ -1519,67 +1656,67 @@
       </c>
     </row>
     <row r="103" spans="1:11">
-      <c r="A103" s="31" t="s">
+      <c r="A103" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B103" s="41"/>
+      <c r="C103" s="41"/>
+      <c r="D103" s="41"/>
+      <c r="E103" s="41"/>
+      <c r="F103" s="11"/>
+      <c r="G103" s="55">
+        <v>0</v>
+      </c>
+      <c r="H103" s="56"/>
+      <c r="I103" s="16">
+        <v>4</v>
+      </c>
+      <c r="J103" s="16">
+        <v>3</v>
+      </c>
+      <c r="K103" s="16">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="A104" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="B103" s="32"/>
-      <c r="C103" s="32"/>
-      <c r="D103" s="32"/>
-      <c r="E103" s="32"/>
-      <c r="F103" s="11"/>
-      <c r="G103" s="53">
-        <v>0</v>
-      </c>
-      <c r="H103" s="54"/>
-      <c r="I103" s="17">
-        <v>4</v>
-      </c>
-      <c r="J103" s="17">
-        <v>3</v>
-      </c>
-      <c r="K103" s="17">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11">
-      <c r="A104" s="46" t="s">
+      <c r="B104" s="43"/>
+      <c r="C104" s="43"/>
+      <c r="D104" s="43"/>
+      <c r="E104" s="43"/>
+      <c r="F104" s="14"/>
+      <c r="G104" s="57"/>
+      <c r="H104" s="58"/>
+      <c r="I104" s="17">
+        <v>10</v>
+      </c>
+      <c r="J104" s="17">
+        <v>2</v>
+      </c>
+      <c r="K104" s="17">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="18.75">
+      <c r="A106" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B104" s="47"/>
-      <c r="C104" s="47"/>
-      <c r="D104" s="47"/>
-      <c r="E104" s="47"/>
-      <c r="F104" s="15"/>
-      <c r="G104" s="55"/>
-      <c r="H104" s="56"/>
-      <c r="I104" s="18">
-        <v>10</v>
-      </c>
-      <c r="J104" s="18">
-        <v>2</v>
-      </c>
-      <c r="K104" s="18">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" ht="18.75">
-      <c r="A106" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B106" s="21"/>
-      <c r="C106" s="22"/>
-      <c r="D106" s="22"/>
-      <c r="E106" s="22"/>
-      <c r="F106" s="22"/>
-      <c r="G106" s="22"/>
-      <c r="H106" s="22"/>
-      <c r="I106" s="22"/>
-      <c r="J106" s="22"/>
-      <c r="K106" s="22"/>
+      <c r="B106" s="20"/>
+      <c r="C106" s="21"/>
+      <c r="D106" s="21"/>
+      <c r="E106" s="21"/>
+      <c r="F106" s="21"/>
+      <c r="G106" s="21"/>
+      <c r="H106" s="21"/>
+      <c r="I106" s="21"/>
+      <c r="J106" s="21"/>
+      <c r="K106" s="21"/>
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
@@ -1587,9 +1724,9 @@
       <c r="E107" s="6"/>
       <c r="F107" s="6"/>
       <c r="G107" s="6"/>
-      <c r="H107" s="23"/>
-      <c r="I107" s="51"/>
-      <c r="J107" s="51"/>
+      <c r="H107" s="22"/>
+      <c r="I107" s="38"/>
+      <c r="J107" s="38"/>
     </row>
     <row r="108" spans="1:11">
       <c r="C108" s="3">
@@ -1605,7 +1742,7 @@
     </row>
     <row r="110" spans="1:11">
       <c r="A110" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="111" spans="1:11">
@@ -1625,12 +1762,12 @@
         <v>2</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="112" spans="1:11">
       <c r="A112" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="113" spans="1:11">
@@ -1654,33 +1791,33 @@
       <c r="F114" s="1"/>
     </row>
     <row r="115" spans="1:11" ht="18.75">
-      <c r="A115" s="24" t="s">
+      <c r="A115" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B115" s="23"/>
+      <c r="C115" s="24"/>
+      <c r="D115" s="24"/>
+      <c r="E115" s="24"/>
+      <c r="F115" s="24"/>
+      <c r="G115" s="24"/>
+      <c r="H115" s="24"/>
+      <c r="I115" s="24"/>
+      <c r="J115" s="24"/>
+      <c r="K115" s="24"/>
+    </row>
+    <row r="116" spans="1:11" ht="31.5" customHeight="1">
+      <c r="A116" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B115" s="24"/>
-      <c r="C115" s="25"/>
-      <c r="D115" s="25"/>
-      <c r="E115" s="25"/>
-      <c r="F115" s="25"/>
-      <c r="G115" s="25"/>
-      <c r="H115" s="25"/>
-      <c r="I115" s="25"/>
-      <c r="J115" s="25"/>
-      <c r="K115" s="25"/>
-    </row>
-    <row r="116" spans="1:11" ht="31.5" customHeight="1">
-      <c r="A116" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="B116" s="50"/>
-      <c r="C116" s="50"/>
-      <c r="D116" s="50"/>
-      <c r="E116" s="50"/>
-      <c r="F116" s="50"/>
-      <c r="G116" s="50"/>
-      <c r="H116" s="50"/>
-      <c r="I116" s="50"/>
-      <c r="J116" s="50"/>
+      <c r="B116" s="37"/>
+      <c r="C116" s="37"/>
+      <c r="D116" s="37"/>
+      <c r="E116" s="37"/>
+      <c r="F116" s="37"/>
+      <c r="G116" s="37"/>
+      <c r="H116" s="37"/>
+      <c r="I116" s="37"/>
+      <c r="J116" s="37"/>
     </row>
     <row r="117" spans="1:11">
       <c r="C117" s="3">
@@ -1691,20 +1828,20 @@
       </c>
       <c r="E117" s="3"/>
       <c r="F117" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G117" s="3">
         <v>1</v>
       </c>
       <c r="H117" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I117" s="6"/>
       <c r="J117" s="6"/>
     </row>
     <row r="119" spans="1:11">
       <c r="A119" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="120" spans="1:11">
@@ -1718,7 +1855,7 @@
         <v>3</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G120" s="6"/>
       <c r="H120" s="6"/>
@@ -1727,7 +1864,7 @@
     </row>
     <row r="122" spans="1:11">
       <c r="A122" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="123" spans="1:11">
@@ -1741,7 +1878,7 @@
         <v>3</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G123" s="6"/>
       <c r="H123" s="6"/>
@@ -1750,7 +1887,7 @@
     </row>
     <row r="125" spans="1:11">
       <c r="A125" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="126" spans="1:11">
@@ -1762,20 +1899,20 @@
       </c>
       <c r="E126" s="3"/>
       <c r="F126" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G126" s="3">
         <v>5</v>
       </c>
       <c r="H126" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I126" s="6"/>
       <c r="J126" s="6"/>
     </row>
     <row r="128" spans="1:11">
       <c r="A128" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="129" spans="1:11">
@@ -1789,7 +1926,7 @@
         <v>3</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G129" s="6"/>
       <c r="H129" s="6"/>
@@ -1797,18 +1934,18 @@
       <c r="J129" s="6"/>
     </row>
     <row r="131" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A131" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="B131" s="49"/>
-      <c r="C131" s="49"/>
-      <c r="D131" s="49"/>
-      <c r="E131" s="49"/>
-      <c r="F131" s="49"/>
-      <c r="G131" s="49"/>
-      <c r="H131" s="49"/>
-      <c r="I131" s="49"/>
-      <c r="J131" s="49"/>
+      <c r="A131" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="B131" s="36"/>
+      <c r="C131" s="36"/>
+      <c r="D131" s="36"/>
+      <c r="E131" s="36"/>
+      <c r="F131" s="36"/>
+      <c r="G131" s="36"/>
+      <c r="H131" s="36"/>
+      <c r="I131" s="36"/>
+      <c r="J131" s="36"/>
     </row>
     <row r="132" spans="1:11">
       <c r="C132" s="3">
@@ -1819,7 +1956,7 @@
       </c>
       <c r="E132" s="3"/>
       <c r="F132" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G132" s="6"/>
       <c r="H132" s="6"/>
@@ -1837,33 +1974,33 @@
       <c r="J133" s="6"/>
     </row>
     <row r="134" spans="1:11" ht="18.75">
-      <c r="A134" s="24" t="s">
+      <c r="A134" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B134" s="23"/>
+      <c r="C134" s="24"/>
+      <c r="D134" s="24"/>
+      <c r="E134" s="24"/>
+      <c r="F134" s="24"/>
+      <c r="G134" s="24"/>
+      <c r="H134" s="24"/>
+      <c r="I134" s="24"/>
+      <c r="J134" s="24"/>
+      <c r="K134" s="24"/>
+    </row>
+    <row r="135" spans="1:11" ht="33" customHeight="1">
+      <c r="A135" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="B134" s="24"/>
-      <c r="C134" s="25"/>
-      <c r="D134" s="25"/>
-      <c r="E134" s="25"/>
-      <c r="F134" s="25"/>
-      <c r="G134" s="25"/>
-      <c r="H134" s="25"/>
-      <c r="I134" s="25"/>
-      <c r="J134" s="25"/>
-      <c r="K134" s="25"/>
-    </row>
-    <row r="135" spans="1:11" ht="33" customHeight="1">
-      <c r="A135" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="B135" s="50"/>
-      <c r="C135" s="50"/>
-      <c r="D135" s="50"/>
-      <c r="E135" s="50"/>
-      <c r="F135" s="50"/>
-      <c r="G135" s="50"/>
-      <c r="H135" s="50"/>
-      <c r="I135" s="50"/>
-      <c r="J135" s="50"/>
+      <c r="B135" s="37"/>
+      <c r="C135" s="37"/>
+      <c r="D135" s="37"/>
+      <c r="E135" s="37"/>
+      <c r="F135" s="37"/>
+      <c r="G135" s="37"/>
+      <c r="H135" s="37"/>
+      <c r="I135" s="37"/>
+      <c r="J135" s="37"/>
     </row>
     <row r="136" spans="1:11">
       <c r="C136" s="3">
@@ -1876,7 +2013,7 @@
         <v>4</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G136" s="6"/>
       <c r="H136" s="6"/>
@@ -1904,18 +2041,18 @@
       <c r="J138" s="6"/>
     </row>
     <row r="139" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A139" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="B139" s="50"/>
-      <c r="C139" s="50"/>
-      <c r="D139" s="50"/>
-      <c r="E139" s="50"/>
-      <c r="F139" s="50"/>
-      <c r="G139" s="50"/>
-      <c r="H139" s="50"/>
-      <c r="I139" s="50"/>
-      <c r="J139" s="50"/>
+      <c r="A139" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B139" s="37"/>
+      <c r="C139" s="37"/>
+      <c r="D139" s="37"/>
+      <c r="E139" s="37"/>
+      <c r="F139" s="37"/>
+      <c r="G139" s="37"/>
+      <c r="H139" s="37"/>
+      <c r="I139" s="37"/>
+      <c r="J139" s="37"/>
     </row>
     <row r="140" spans="1:11">
       <c r="C140" s="3">
@@ -1928,7 +2065,7 @@
         <v>1</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G140" s="6"/>
       <c r="H140" s="6"/>
@@ -1936,33 +2073,33 @@
       <c r="J140" s="6"/>
     </row>
     <row r="141" spans="1:11" ht="18.75">
-      <c r="A141" s="24" t="s">
+      <c r="A141" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B141" s="23"/>
+      <c r="C141" s="24"/>
+      <c r="D141" s="24"/>
+      <c r="E141" s="24"/>
+      <c r="F141" s="24"/>
+      <c r="G141" s="24"/>
+      <c r="H141" s="24"/>
+      <c r="I141" s="24"/>
+      <c r="J141" s="24"/>
+      <c r="K141" s="24"/>
+    </row>
+    <row r="142" spans="1:11" ht="61.5" customHeight="1">
+      <c r="A142" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="B141" s="24"/>
-      <c r="C141" s="25"/>
-      <c r="D141" s="25"/>
-      <c r="E141" s="25"/>
-      <c r="F141" s="25"/>
-      <c r="G141" s="25"/>
-      <c r="H141" s="25"/>
-      <c r="I141" s="25"/>
-      <c r="J141" s="25"/>
-      <c r="K141" s="25"/>
-    </row>
-    <row r="142" spans="1:11" ht="61.5" customHeight="1">
-      <c r="A142" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="B142" s="49"/>
-      <c r="C142" s="49"/>
-      <c r="D142" s="49"/>
-      <c r="E142" s="49"/>
-      <c r="F142" s="49"/>
-      <c r="G142" s="49"/>
-      <c r="H142" s="49"/>
-      <c r="I142" s="49"/>
-      <c r="J142" s="49"/>
+      <c r="B142" s="36"/>
+      <c r="C142" s="36"/>
+      <c r="D142" s="36"/>
+      <c r="E142" s="36"/>
+      <c r="F142" s="36"/>
+      <c r="G142" s="36"/>
+      <c r="H142" s="36"/>
+      <c r="I142" s="36"/>
+      <c r="J142" s="36"/>
     </row>
     <row r="143" spans="1:11">
       <c r="C143" s="3">
@@ -1975,7 +2112,7 @@
         <v>2</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G143" s="6"/>
       <c r="H143" s="6"/>
@@ -1984,7 +2121,7 @@
     </row>
     <row r="145" spans="1:10">
       <c r="A145" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="146" spans="1:10">
@@ -1992,7 +2129,7 @@
       <c r="B146" s="6"/>
       <c r="C146" s="3"/>
       <c r="D146" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E146" s="6"/>
       <c r="F146" s="10"/>
@@ -2008,7 +2145,7 @@
         <v>1</v>
       </c>
       <c r="D147" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E147" s="6"/>
       <c r="F147" s="10"/>
@@ -2022,7 +2159,7 @@
       <c r="B148" s="6"/>
       <c r="C148" s="3"/>
       <c r="D148" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E148" s="6"/>
       <c r="F148" s="10"/>
@@ -2038,7 +2175,7 @@
         <v>5</v>
       </c>
       <c r="D149" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E149" s="6"/>
       <c r="F149" s="10"/>
@@ -2048,18 +2185,18 @@
       <c r="J149" s="6"/>
     </row>
     <row r="151" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A151" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="B151" s="50"/>
-      <c r="C151" s="50"/>
-      <c r="D151" s="50"/>
-      <c r="E151" s="50"/>
-      <c r="F151" s="50"/>
-      <c r="G151" s="50"/>
-      <c r="H151" s="50"/>
-      <c r="I151" s="50"/>
-      <c r="J151" s="50"/>
+      <c r="A151" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B151" s="37"/>
+      <c r="C151" s="37"/>
+      <c r="D151" s="37"/>
+      <c r="E151" s="37"/>
+      <c r="F151" s="37"/>
+      <c r="G151" s="37"/>
+      <c r="H151" s="37"/>
+      <c r="I151" s="37"/>
+      <c r="J151" s="37"/>
     </row>
     <row r="152" spans="1:10">
       <c r="C152" s="3">
@@ -2072,7 +2209,7 @@
         <v>2</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G152" s="6"/>
       <c r="H152" s="6"/>
@@ -2080,40 +2217,9 @@
       <c r="J152" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="A139:J139"/>
-    <mergeCell ref="A142:J142"/>
-    <mergeCell ref="A151:J151"/>
-    <mergeCell ref="I107:J107"/>
-    <mergeCell ref="A116:J116"/>
-    <mergeCell ref="A131:J131"/>
-    <mergeCell ref="A135:J135"/>
-    <mergeCell ref="A103:E103"/>
-    <mergeCell ref="A104:E104"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="A101:F101"/>
-    <mergeCell ref="G101:H101"/>
-    <mergeCell ref="I101:K101"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="G102:H102"/>
-    <mergeCell ref="G103:H103"/>
-    <mergeCell ref="G104:H104"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="J60:K60"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A56:E56"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="I53:K53"/>
+  <mergeCells count="33">
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A13:E13"/>
-    <mergeCell ref="J15:K15"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="A9:E9"/>
@@ -2122,6 +2228,29 @@
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="I53:K53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A56:E56"/>
+    <mergeCell ref="A103:E103"/>
+    <mergeCell ref="A104:E104"/>
+    <mergeCell ref="A101:F101"/>
+    <mergeCell ref="G101:H101"/>
+    <mergeCell ref="I101:K101"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="G102:H102"/>
+    <mergeCell ref="G103:H103"/>
+    <mergeCell ref="G104:H104"/>
+    <mergeCell ref="A139:J139"/>
+    <mergeCell ref="A142:J142"/>
+    <mergeCell ref="A151:J151"/>
+    <mergeCell ref="I107:J107"/>
+    <mergeCell ref="A116:J116"/>
+    <mergeCell ref="A131:J131"/>
+    <mergeCell ref="A135:J135"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>